<commit_message>
Release Revision 1-0 of project 8307 RF Power Sensor
</commit_message>
<xml_diff>
--- a/RF Power Detectors - comparație.xlsx
+++ b/RF Power Detectors - comparație.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/KiCAD/00 Proiecte/8307 RF Power Sensor Rev1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6BAB3C-C128-E94B-B800-EE1BEE84FEE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036087F5-A1C6-A44C-9147-E6C1AC52B733}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7281C468-C2AB-234A-BDAE-24A266A097CF}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>LTC5507</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>envelope + RMS</t>
+  </si>
+  <si>
+    <t>AD8319</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_)\ _R_O_N_ ;_ * \(#,##0.00\)\ _R_O_N_ ;_ * &quot;-&quot;??_)\ _R_O_N_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,13 +161,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -537,7 +533,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -654,6 +650,9 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>

</xml_diff>